<commit_message>
Mise à jour des données 03/12/18
</commit_message>
<xml_diff>
--- a/data-raw/Inscription.xlsx
+++ b/data-raw/Inscription.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="269">
   <si>
     <t>CSP parents (code)</t>
   </si>
@@ -39,12 +39,6 @@
     <t>agric. M.E</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>agric. G.E</t>
-  </si>
-  <si>
     <t>21</t>
   </si>
   <si>
@@ -309,6 +303,12 @@
     <t>Profil étudiant (lib.)</t>
   </si>
   <si>
+    <t>2D</t>
+  </si>
+  <si>
+    <t>UPS D2E</t>
+  </si>
+  <si>
     <t>2E</t>
   </si>
   <si>
@@ -649,6 +649,12 @@
   </si>
   <si>
     <t>cotutelle</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>TH seule</t>
   </si>
   <si>
     <t>X1</t>
@@ -930,7 +936,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView rightToLeft="0" workbookViewId="0"/>
   </sheetViews>
@@ -1317,15 +1323,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B49" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+    <row r="49" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
@@ -1334,7 +1332,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView rightToLeft="0" workbookViewId="0"/>
   </sheetViews>
@@ -1348,439 +1346,439 @@
     <row r="1" s="1" customFormat="1" ht="12.2659" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B9" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B10" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B11" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B12" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B13" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B14" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B15" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B16" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B17" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B18" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B19" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B20" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B21" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B22" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B23" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B24" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B25" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B26" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B27" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B28" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B29" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B30" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B31" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B32" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B33" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B34" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B35" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>99</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B36" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B37" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B38" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B39" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B40" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B41" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B42" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B43" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B44" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B45" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B46" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="47" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B47" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B48" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="49" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B49" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B50" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B51" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B52" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="53" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B53" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B54" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="55" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B55" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="56" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B56" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>201</v>
@@ -1788,53 +1786,69 @@
     </row>
     <row r="57" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B57" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="58" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B58" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="59" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B59" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="60" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B60" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="61" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B61" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B62" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="63" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B63" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C63" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="63" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+    <row r="64" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B64" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="65" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
@@ -1856,58 +1870,58 @@
     <row r="1" s="1" customFormat="1" ht="14.3991" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
@@ -1932,39 +1946,39 @@
     <row r="1" s="1" customFormat="1" ht="14.9324" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>128</v>
@@ -1972,26 +1986,26 @@
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B9" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
@@ -2016,58 +2030,58 @@
     <row r="1" s="1" customFormat="1" ht="4.2664" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="11.1993" customHeight="1">
@@ -2097,26 +2111,26 @@
     <row r="1" s="1" customFormat="1" ht="86.3946" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
@@ -2124,15 +2138,15 @@
         <v>117</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
@@ -2140,31 +2154,31 @@
         <v>174</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B9" s="3" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B10" s="4" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" ht="19.7321" customHeight="1">
@@ -2172,7 +2186,7 @@
         <v>205</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" ht="28.7982" customHeight="1"/>

</xml_diff>

<commit_message>
Mise à jour Apogée (13 février 2019)
</commit_message>
<xml_diff>
--- a/data-raw/Inscription.xlsx
+++ b/data-raw/Inscription.xlsx
@@ -39,6 +39,12 @@
     <t>agric. M.E</t>
   </si>
   <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>agric. G.E</t>
+  </si>
+  <si>
     <t>21</t>
   </si>
   <si>
@@ -301,12 +307,6 @@
   </si>
   <si>
     <t>Profil étudiant (lib.)</t>
-  </si>
-  <si>
-    <t>2D</t>
-  </si>
-  <si>
-    <t>UPS D2E</t>
   </si>
   <si>
     <t>2E</t>
@@ -936,7 +936,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C50"/>
   <cols>
     <col min="1" max="1" width="25.9535986666667" customWidth="1"/>
     <col min="2" max="3" width="10.7163133333333" customWidth="1"/>
@@ -1320,7 +1320,15 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+    <row r="49" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B49" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
@@ -1329,7 +1337,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C64"/>
   <cols>
     <col min="1" max="1" width="20.5347986666667" customWidth="1"/>
     <col min="2" max="2" width="10.7163133333333" customWidth="1"/>
@@ -1340,439 +1348,439 @@
     <row r="1" s="1" customFormat="1" ht="12.2659" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B9" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B10" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B11" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B12" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B13" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B14" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B15" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B16" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B17" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B18" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B19" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B20" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B21" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B22" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B23" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B24" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B25" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B26" s="4" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B27" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B28" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B29" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B30" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B31" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B32" s="4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B33" s="3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B34" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B35" s="3" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>160</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B36" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>99</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B37" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B38" s="4" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B39" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B40" s="4" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B41" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B42" s="4" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B43" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B44" s="4" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="45" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B45" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B46" s="4" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="47" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B47" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="48" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B48" s="4" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="49" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B49" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B50" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B51" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="52" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B52" s="4" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="53" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B53" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="54" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B54" s="4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="55" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B55" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="56" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B56" s="4" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>201</v>
@@ -1780,69 +1788,61 @@
     </row>
     <row r="57" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B57" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="58" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B58" s="4" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="59" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B59" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="60" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B60" s="4" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="61" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B61" s="3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B62" s="4" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="63" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B63" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="64" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B64" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="C64" s="4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="65" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+    <row r="64" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
Mise à jour apogée mars2019
</commit_message>
<xml_diff>
--- a/data-raw/Inscription.xlsx
+++ b/data-raw/Inscription.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="271">
   <si>
     <t>CSP parents (code)</t>
   </si>
@@ -307,6 +307,12 @@
   </si>
   <si>
     <t>Profil étudiant (lib.)</t>
+  </si>
+  <si>
+    <t>2D</t>
+  </si>
+  <si>
+    <t>UPS D2E</t>
   </si>
   <si>
     <t>2E</t>
@@ -1337,7 +1343,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C65"/>
   <cols>
     <col min="1" max="1" width="20.5347986666667" customWidth="1"/>
     <col min="2" max="2" width="10.7163133333333" customWidth="1"/>
@@ -1383,15 +1389,15 @@
         <v>104</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
@@ -1615,15 +1621,15 @@
         <v>161</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>99</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B36" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>163</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" ht="19.7321" customHeight="1">
@@ -1783,15 +1789,15 @@
         <v>202</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="57" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B57" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="58" s="1" customFormat="1" ht="19.7321" customHeight="1">
@@ -1799,15 +1805,15 @@
         <v>205</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B59" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="60" s="1" customFormat="1" ht="19.7321" customHeight="1">
@@ -1842,7 +1848,15 @@
         <v>215</v>
       </c>
     </row>
-    <row r="64" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+    <row r="64" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B64" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="65" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
@@ -1861,58 +1875,58 @@
     <row r="1" s="1" customFormat="1" ht="14.3991" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
@@ -1934,66 +1948,66 @@
     <row r="1" s="1" customFormat="1" ht="14.9324" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B9" s="3" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
@@ -2015,58 +2029,58 @@
     <row r="1" s="1" customFormat="1" ht="4.2664" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="11.1993" customHeight="1">
@@ -2093,82 +2107,82 @@
     <row r="1" s="1" customFormat="1" ht="86.3946" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B9" s="3" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B10" s="4" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B11" s="3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" ht="28.7982" customHeight="1"/>

</xml_diff>

<commit_message>
Maj apogée juillet 2019
</commit_message>
<xml_diff>
--- a/data-raw/Inscription.xlsx
+++ b/data-raw/Inscription.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="263">
   <si>
     <t>CSP parents (code)</t>
   </si>
@@ -27,6 +27,24 @@
     <t>agriculteu</t>
   </si>
   <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>agric. P.E</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>agric. M.E</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>agric. G.E</t>
+  </si>
+  <si>
     <t>21</t>
   </si>
   <si>
@@ -159,12 +177,48 @@
     <t>ouvrier q</t>
   </si>
   <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>ouv. Q.Ind</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>ouv. Q.art</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>chauffeurs</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>ouv. Q. ma</t>
+  </si>
+  <si>
     <t>66</t>
   </si>
   <si>
     <t>ouvrier nq</t>
   </si>
   <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>ouv. NQI</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>ouv. NQA</t>
+  </si>
+  <si>
     <t>69</t>
   </si>
   <si>
@@ -189,12 +243,36 @@
     <t>retrait cd</t>
   </si>
   <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>ret. CAD</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>ret. PI</t>
+  </si>
+  <si>
     <t>76</t>
   </si>
   <si>
     <t>retrait em</t>
   </si>
   <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>ret. emp.</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>ret. ouv</t>
+  </si>
+  <si>
     <t>81</t>
   </si>
   <si>
@@ -207,6 +285,18 @@
     <t>ss act pro</t>
   </si>
   <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>ss pro.-60</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>ss pro+60</t>
+  </si>
+  <si>
     <t>99</t>
   </si>
   <si>
@@ -219,6 +309,24 @@
     <t>Profil étudiant (lib.)</t>
   </si>
   <si>
+    <t>2D</t>
+  </si>
+  <si>
+    <t>UPS D2E</t>
+  </si>
+  <si>
+    <t>2E</t>
+  </si>
+  <si>
+    <t>Etud. entr</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>auditeur</t>
+  </si>
+  <si>
     <t>AE</t>
   </si>
   <si>
@@ -228,9 +336,6 @@
     <t>AL</t>
   </si>
   <si>
-    <t>auditeur</t>
-  </si>
-  <si>
     <t>AS</t>
   </si>
   <si>
@@ -249,6 +354,36 @@
     <t>capacite</t>
   </si>
   <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Cés. payée</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>Césure 1/2</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>Césure exo</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>chg etb</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>cohab.int.</t>
+  </si>
+  <si>
     <t>CO</t>
   </si>
   <si>
@@ -273,10 +408,10 @@
     <t>internat</t>
   </si>
   <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>di-disport</t>
+    <t>DL</t>
+  </si>
+  <si>
+    <t>dip-lv-drt</t>
   </si>
   <si>
     <t>DU</t>
@@ -297,12 +432,6 @@
     <t>thèssan E1</t>
   </si>
   <si>
-    <t>E2</t>
-  </si>
-  <si>
-    <t>thèssan E2</t>
-  </si>
-  <si>
     <t>EC</t>
   </si>
   <si>
@@ -363,12 +492,27 @@
     <t>IFSI</t>
   </si>
   <si>
+    <t>JD</t>
+  </si>
+  <si>
     <t>LP</t>
   </si>
   <si>
     <t>Lic. Prof.</t>
   </si>
   <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>UFR LV+SS</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>mobilité</t>
+  </si>
+  <si>
     <t>ME</t>
   </si>
   <si>
@@ -381,6 +525,12 @@
     <t>mont-nul</t>
   </si>
   <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>mobil.+SS</t>
+  </si>
+  <si>
     <t>NO</t>
   </si>
   <si>
@@ -423,6 +573,18 @@
     <t>Réorient I</t>
   </si>
   <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>Remediat.</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>Ex-Et-SS</t>
+  </si>
+  <si>
     <t>SF</t>
   </si>
   <si>
@@ -450,6 +612,12 @@
     <t>T2</t>
   </si>
   <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>cotute. P.</t>
+  </si>
+  <si>
     <t>TH</t>
   </si>
   <si>
@@ -471,6 +639,12 @@
     <t>cotutelle</t>
   </si>
   <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>Exo.BFMP</t>
+  </si>
+  <si>
     <t>Régime d'inscription (code)</t>
   </si>
   <si>
@@ -585,16 +759,25 @@
     <t>Situation sociale (lib.)</t>
   </si>
   <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>Bours CPGE</t>
+  </si>
+  <si>
     <t>BO</t>
   </si>
   <si>
     <t>Boursier</t>
   </si>
   <si>
-    <t>CH</t>
-  </si>
-  <si>
     <t>Chomeur</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>Demi Droit</t>
   </si>
   <si>
     <t>Normal</t>
@@ -735,7 +918,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C50"/>
   <cols>
     <col min="1" max="1" width="25.9535986666667" customWidth="1"/>
     <col min="2" max="3" width="10.7163133333333" customWidth="1"/>
@@ -1007,7 +1190,127 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+    <row r="35" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B36" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B37" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B38" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B39" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B40" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B41" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B42" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B43" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B44" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B45" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B46" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B47" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B48" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B49" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
@@ -1016,7 +1319,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C61"/>
   <cols>
     <col min="1" max="1" width="20.5347986666667" customWidth="1"/>
     <col min="2" max="2" width="10.7163133333333" customWidth="1"/>
@@ -1027,357 +1330,477 @@
     <row r="1" s="1" customFormat="1" ht="12.2659" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B9" s="3" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B10" s="4" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B11" s="3" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B12" s="4" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B13" s="3" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B14" s="4" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B15" s="3" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B16" s="4" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B17" s="3" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>97</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B18" s="4" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B19" s="3" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>101</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B20" s="4" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>103</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B21" s="3" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B22" s="4" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B23" s="3" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>109</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B24" s="4" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B25" s="3" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B26" s="4" t="s">
-        <v>114</v>
+        <v>143</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>115</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B27" s="3" t="s">
-        <v>116</v>
+        <v>145</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B28" s="4" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B29" s="3" t="s">
-        <v>120</v>
+        <v>149</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>121</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B30" s="4" t="s">
-        <v>122</v>
+        <v>151</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B31" s="3" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>125</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B32" s="4" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>127</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B33" s="3" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B34" s="4" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B35" s="3" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B36" s="4" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B37" s="3" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B38" s="4" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B39" s="3" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B40" s="4" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B41" s="3" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>143</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B42" s="4" t="s">
-        <v>145</v>
+        <v>174</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B43" s="3" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B44" s="4" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
     </row>
     <row r="45" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B45" s="3" t="s">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="46" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B46" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B47" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="48" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B48" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B49" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="50" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B50" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B51" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="52" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B52" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="53" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B53" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="54" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B54" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="55" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B55" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="56" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B56" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="57" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B57" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="58" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B58" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="59" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B59" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="60" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B60" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="61" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
@@ -1396,58 +1819,58 @@
     <row r="1" s="1" customFormat="1" ht="14.3991" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>152</v>
+        <v>210</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>153</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>154</v>
+        <v>212</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>155</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>156</v>
+        <v>214</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>157</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>158</v>
+        <v>216</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>159</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>160</v>
+        <v>218</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>161</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>162</v>
+        <v>220</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>163</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>164</v>
+        <v>222</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>165</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
@@ -1469,66 +1892,66 @@
     <row r="1" s="1" customFormat="1" ht="14.9324" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>166</v>
+        <v>224</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>167</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>168</v>
+        <v>226</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>169</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>170</v>
+        <v>228</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>171</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>172</v>
+        <v>230</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>173</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>174</v>
+        <v>232</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>175</v>
+        <v>233</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>176</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>177</v>
+        <v>235</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>178</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B9" s="3" t="s">
-        <v>179</v>
+        <v>237</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>180</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
@@ -1540,7 +1963,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <cols>
     <col min="1" max="1" width="30.6613" customWidth="1"/>
     <col min="2" max="3" width="10.7163133333333" customWidth="1"/>
@@ -1550,57 +1973,65 @@
     <row r="1" s="1" customFormat="1" ht="4.2664" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>181</v>
+        <v>239</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>182</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>168</v>
+        <v>226</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>183</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>170</v>
+        <v>228</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>184</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>172</v>
+        <v>230</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>185</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>174</v>
+        <v>232</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>186</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>175</v>
+        <v>233</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="8" s="1" customFormat="1" ht="11.1993" customHeight="1">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B8" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="11.1993" customHeight="1">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
@@ -1609,7 +2040,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <cols>
     <col min="1" max="1" width="36.0801" customWidth="1"/>
     <col min="2" max="2" width="10.7163133333333" customWidth="1"/>
@@ -1620,69 +2051,85 @@
     <row r="1" s="1" customFormat="1" ht="86.3946" customHeight="1"/>
     <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>188</v>
+        <v>246</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>189</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>190</v>
+        <v>248</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>191</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>192</v>
+        <v>250</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>193</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>194</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>195</v>
+        <v>253</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>196</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>198</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>199</v>
+        <v>256</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>200</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B9" s="3" t="s">
-        <v>145</v>
+        <v>258</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B10" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B11" s="3" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="10" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+      <c r="C11" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>